<commit_message>
Scenariusz rejestracja + dodane dwóch kroków w Logowanie
</commit_message>
<xml_diff>
--- a/test scripts.xlsx
+++ b/test scripts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Menu i zakładki" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -65,16 +65,89 @@
     <t>Sprawdza czy wyskakuje "Podałeś błędne dane logowania". Sprawdzenie czy imputy puste.</t>
   </si>
   <si>
-    <t>Poprawne logowanie na ADMINA.</t>
-  </si>
-  <si>
     <t>Sprawdza czy widoczna jest zakładka "Dodaj książkę"</t>
   </si>
   <si>
-    <t>Poprawne logowanie na USER.</t>
-  </si>
-  <si>
     <t>Sprawdza czy NIE widoczna jest zakładka "Dodaj książkę"</t>
+  </si>
+  <si>
+    <t>Rejestracja z pustymi polami</t>
+  </si>
+  <si>
+    <t>Sprawdzenie czy wyskakuje:
+"6 errors
+    Username can't be blank
+    Username is too short (minimum is 3 characters)
+    Email can't be blank
+    Email is invalid
+    Password can't be blank
+    Password is invalid"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rejestracja jedynie z Nazwa Użytkownika </t>
+  </si>
+  <si>
+    <t>Rejestracja jedynie z Nazwa Użytkownika (Lenght&lt; 3)</t>
+  </si>
+  <si>
+    <t>Rejestracja jedynie z mailem</t>
+  </si>
+  <si>
+    <t>Sprawdza czy wyskakuje: 
+4 errors
+    Username can't be blank
+    Username is too short (minimum is 3 characters)
+    Password can't be blank
+    Password is invalid"</t>
+  </si>
+  <si>
+    <t>Sprawdzenie czy wyskakuje:
+"4 errors
+    Email can't be blank
+    Email is invalid
+    Password can't be blank
+    Password is invalid"</t>
+  </si>
+  <si>
+    <t>Sprawdzenie czy wyskakuje:
+"5 errors
+    Username is too short (minimum is 3 characters)
+    Email can't be blank
+    Email is invalid
+    Password can't be blank
+    Password is invalid"</t>
+  </si>
+  <si>
+    <t>Rejestracja istniejący użytkownik+mail+hasło</t>
+  </si>
+  <si>
+    <t>Sprawdza czy wyskakuje:
+"Username has already been taken"</t>
+  </si>
+  <si>
+    <t>Rejestracja użytkownik+ istniejący mail+hasło</t>
+  </si>
+  <si>
+    <t>Rejestracja poprawna użytkownik+ mail+hasło</t>
+  </si>
+  <si>
+    <t>Sprawdza czy wyskakuje: 
+"Email  has already been taken"</t>
+  </si>
+  <si>
+    <t>Sprawdzanie czy rejestracja przebiegła poprawnie</t>
+  </si>
+  <si>
+    <t>Poprawne logowanie na ADMINA za pomocą Loginu.</t>
+  </si>
+  <si>
+    <t>Poprawne logowanie na USER  za pomocą Loginu.</t>
+  </si>
+  <si>
+    <t>Poprawne logowanie na ADMINA za pomocą Maila.</t>
+  </si>
+  <si>
+    <t>Poprawne logowanie na USER  za pomocą Maila.</t>
   </si>
 </sst>
 </file>
@@ -110,13 +183,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -144,14 +242,28 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A1:E6" totalsRowShown="0">
-  <autoFilter ref="A1:E6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A1:E8" totalsRowShown="0">
+  <autoFilter ref="A1:E8"/>
   <tableColumns count="5">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Opis kroku"/>
     <tableColumn id="3" name="Weryfikacja"/>
     <tableColumn id="4" name="Czy działa"/>
     <tableColumn id="5" name="Odpowiedzialny"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela32" displayName="Tabela32" ref="A1:E8" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:E8"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="ID" dataDxfId="5"/>
+    <tableColumn id="2" name="Opis kroku" dataDxfId="4"/>
+    <tableColumn id="3" name="Weryfikacja" dataDxfId="3"/>
+    <tableColumn id="4" name="Czy działa" dataDxfId="2"/>
+    <tableColumn id="5" name="Odpowiedzialny" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -475,15 +587,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
@@ -553,10 +665,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -567,12 +679,40 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -586,12 +726,144 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Wrzucenie nowych scenariuszy do nowego arkusza
</commit_message>
<xml_diff>
--- a/test scripts.xlsx
+++ b/test scripts.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19401"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCAE41C0-0EB2-45E8-A7EC-B1BE82E6BC4C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Menu i zakładki" sheetId="2" r:id="rId1"/>
     <sheet name="Logowanie" sheetId="1" r:id="rId2"/>
     <sheet name="Rejestracja" sheetId="3" r:id="rId3"/>
+    <sheet name="OcenaOpinia" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179016"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -193,8 +193,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,16 +202,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor theme="8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -219,16 +239,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -268,42 +330,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="A1:E2" totalsRowShown="0">
-  <autoFilter ref="A1:E2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:E2" totalsRowShown="0">
+  <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Opis kroku"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Weryfikacja"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Czy działa"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Odpowiedzialny"/>
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="Opis kroku"/>
+    <tableColumn id="3" name="Weryfikacja"/>
+    <tableColumn id="4" name="Czy działa"/>
+    <tableColumn id="5" name="Odpowiedzialny"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela3" displayName="Tabela3" ref="A1:E8" totalsRowShown="0">
-  <autoFilter ref="A1:E8" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A1:E8" totalsRowShown="0">
+  <autoFilter ref="A1:E8"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Opis kroku"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Weryfikacja"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Czy działa"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Odpowiedzialny"/>
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="Opis kroku"/>
+    <tableColumn id="3" name="Weryfikacja"/>
+    <tableColumn id="4" name="Czy działa"/>
+    <tableColumn id="5" name="Odpowiedzialny"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabela32" displayName="Tabela32" ref="A1:E15" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela32" displayName="Tabela32" ref="A1:E8" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E8"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ID" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Opis kroku" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Weryfikacja" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Czy działa" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Odpowiedzialny" dataDxfId="0"/>
+    <tableColumn id="1" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" name="Opis kroku" dataDxfId="3"/>
+    <tableColumn id="3" name="Weryfikacja" dataDxfId="2"/>
+    <tableColumn id="4" name="Czy działa" dataDxfId="1"/>
+    <tableColumn id="5" name="Odpowiedzialny" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -571,14 +633,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="74.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.85546875" bestFit="1" customWidth="1"/>
@@ -586,7 +648,7 @@
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -603,7 +665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -626,22 +688,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -658,7 +720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -672,7 +734,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -686,7 +748,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -700,7 +762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -714,7 +776,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -728,7 +790,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -742,7 +804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -765,22 +827,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
-      <selection activeCell="E9" sqref="E9:E15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -797,7 +859,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="120">
+    <row r="2" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -812,7 +874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="105">
+    <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -827,7 +889,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="90">
+    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -842,7 +904,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="90">
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -857,7 +919,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -872,7 +934,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -887,7 +949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -900,111 +962,6 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="2">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30">
-      <c r="A11" s="2">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="2">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30">
-      <c r="A13" s="2">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30">
-      <c r="A14" s="2">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30">
-      <c r="A15" s="2">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1013,4 +970,146 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.140625" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Wspólne REPO+ Poprawiona instrukcja
</commit_message>
<xml_diff>
--- a/test scripts.xlsx
+++ b/test scripts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Menu i zakładki" sheetId="2" r:id="rId1"/>
@@ -830,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,7 +976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1019,7 +1019,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Wszystkie zmienne (Login,Mail,Pass) w REPO. Testy Rejestracji skończone.
</commit_message>
<xml_diff>
--- a/test scripts.xlsx
+++ b/test scripts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -188,6 +188,15 @@
   </si>
   <si>
     <t>Sprawdzenie opinii innego użytkownika jako admin - istnieją opinie</t>
+  </si>
+  <si>
+    <t>Rejestracja istniejący użytkownik+ istniejący mail+ hasło</t>
+  </si>
+  <si>
+    <t>Sprawdza czy wyskakuje:
+2 errors
+    Username has already been taken
+    Email has already been taken</t>
   </si>
 </sst>
 </file>
@@ -358,8 +367,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela32" displayName="Tabela32" ref="A1:E8" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela32" displayName="Tabela32" ref="A1:E9" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E9"/>
   <tableColumns count="5">
     <tableColumn id="1" name="ID" dataDxfId="4"/>
     <tableColumn id="2" name="Opis kroku" dataDxfId="3"/>
@@ -828,15 +837,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" customWidth="1"/>
     <col min="3" max="3" width="46.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
@@ -876,7 +885,7 @@
     </row>
     <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>22</v>
@@ -891,7 +900,7 @@
     </row>
     <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>24</v>
@@ -919,15 +928,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
@@ -936,31 +945,46 @@
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Prawie skończona rejestracja. Do dokończenia kasowanie usera testowego.
</commit_message>
<xml_diff>
--- a/test scripts.xlsx
+++ b/test scripts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Menu i zakładki" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Odpowiedzialny</t>
-  </si>
-  <si>
-    <t>Sprawdzenie wszystkich kontolek (input, label, button) na wszystkich zakładkach.</t>
   </si>
   <si>
     <t>Sprawdzenie czy wszystkie kontrolki we wszytkich zakładkach są wyswietlane.</t>
@@ -197,6 +194,15 @@
 2 errors
     Username has already been taken
     Email has already been taken</t>
+  </si>
+  <si>
+    <t>Sprawdzenie wszystkich kontolek (input, label, button) na wszystkich zakładkach przed zalogowaniem.</t>
+  </si>
+  <si>
+    <t>Sprawdzenie wszystkich kontolek (input, label, button) na wszystkich zakładkach jako User.</t>
+  </si>
+  <si>
+    <t>Sprawdzenie wszystkich kontolek (input, label, button) na wszystkich zakładkach jako Admin.</t>
   </si>
 </sst>
 </file>
@@ -339,8 +345,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:E2" totalsRowShown="0">
-  <autoFilter ref="A1:E2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:E4" totalsRowShown="0">
+  <autoFilter ref="A1:E4"/>
   <tableColumns count="5">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Opis kroku"/>
@@ -643,15 +649,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="74.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
@@ -679,13 +685,41 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -734,13 +768,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -748,13 +782,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -762,13 +796,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -776,13 +810,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -790,13 +824,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -804,13 +838,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -818,13 +852,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -839,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,14 +907,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -888,14 +922,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -903,89 +937,89 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1033,14 +1067,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1048,14 +1082,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1063,14 +1097,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1078,14 +1112,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1093,14 +1127,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1108,14 +1142,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1123,14 +1157,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rozpoczęcie testów wszystkich kontrolek (niezalogowany)
</commit_message>
<xml_diff>
--- a/test scripts.xlsx
+++ b/test scripts.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19406"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA13CC18-D7DD-4C45-9DDE-A15C5523D9F0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Menu i zakładki" sheetId="2" r:id="rId1"/>
@@ -13,7 +12,7 @@
     <sheet name="Rejestracja" sheetId="3" r:id="rId3"/>
     <sheet name="OcenaOpinia" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179016"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -233,8 +232,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,42 +402,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="A1:E4" totalsRowShown="0">
-  <autoFilter ref="A1:E4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:E4" totalsRowShown="0">
+  <autoFilter ref="A1:E4"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Opis kroku"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Weryfikacja"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Czy działa"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Odpowiedzialny"/>
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="Opis kroku"/>
+    <tableColumn id="3" name="Weryfikacja"/>
+    <tableColumn id="4" name="Czy działa"/>
+    <tableColumn id="5" name="Odpowiedzialny"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela3" displayName="Tabela3" ref="A1:E8" totalsRowShown="0">
-  <autoFilter ref="A1:E8" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A1:E8" totalsRowShown="0">
+  <autoFilter ref="A1:E8"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Opis kroku"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Weryfikacja"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Czy działa"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Odpowiedzialny"/>
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="Opis kroku"/>
+    <tableColumn id="3" name="Weryfikacja"/>
+    <tableColumn id="4" name="Czy działa"/>
+    <tableColumn id="5" name="Odpowiedzialny"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabela32" displayName="Tabela32" ref="A1:E9" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela32" displayName="Tabela32" ref="A1:E9" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E9"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ID" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Opis kroku" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Weryfikacja" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Czy działa" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Odpowiedzialny" dataDxfId="0"/>
+    <tableColumn id="1" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" name="Opis kroku" dataDxfId="3"/>
+    <tableColumn id="3" name="Weryfikacja" dataDxfId="2"/>
+    <tableColumn id="4" name="Czy działa" dataDxfId="1"/>
+    <tableColumn id="5" name="Odpowiedzialny" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -706,14 +705,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="93.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.85546875" bestFit="1" customWidth="1"/>
@@ -721,7 +720,7 @@
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -738,7 +737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -752,7 +751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -766,7 +765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -789,14 +788,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="48.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.7109375" bestFit="1" customWidth="1"/>
@@ -804,7 +803,7 @@
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -821,7 +820,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -835,7 +834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -849,7 +848,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -863,7 +862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -877,7 +876,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -891,7 +890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -905,7 +904,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -928,14 +927,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="54.140625" customWidth="1"/>
     <col min="3" max="3" width="46.42578125" bestFit="1" customWidth="1"/>
@@ -943,7 +942,7 @@
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -960,7 +959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="120">
+    <row r="2" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -975,7 +974,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="105">
+    <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -990,7 +989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="90">
+    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1005,7 +1004,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="90">
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1020,7 +1019,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="75">
+    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1035,7 +1034,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1050,7 +1049,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1065,7 +1064,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1089,14 +1088,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.140625" customWidth="1"/>
@@ -1105,7 +1104,7 @@
     <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1122,7 +1121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1137,7 +1136,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1152,7 +1151,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1167,7 +1166,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1182,7 +1181,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1197,7 +1196,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1212,7 +1211,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -1227,7 +1226,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1242,7 +1241,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -1257,7 +1256,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -1272,21 +1271,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>

</xml_diff>

<commit_message>
Dodanie próbu usunięcia admina (Rejestracja)
</commit_message>
<xml_diff>
--- a/test scripts.xlsx
+++ b/test scripts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Menu i zakładki" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
@@ -227,6 +227,13 @@
   </si>
   <si>
     <t>Sprawdzenie, czy wyświetlana jest właściwa średnia ocen</t>
+  </si>
+  <si>
+    <t>Próba usunięcia konta admina</t>
+  </si>
+  <si>
+    <t>Sprawdza czy wyskakuje: 
+"Nie możesz usunąć administratora"</t>
   </si>
 </sst>
 </file>
@@ -430,8 +437,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela32" displayName="Tabela32" ref="A1:E9" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela32" displayName="Tabela32" ref="A1:E10" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E10"/>
   <tableColumns count="5">
     <tableColumn id="1" name="ID" dataDxfId="4"/>
     <tableColumn id="2" name="Opis kroku" dataDxfId="3"/>
@@ -708,7 +715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -928,10 +935,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,6 +1086,21 @@
         <v>7</v>
       </c>
     </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1091,9 +1113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>